<commit_message>
Send excel to sharepoint
</commit_message>
<xml_diff>
--- a/src/main/resources/imports/docs/munkalap_sablon_uj.xlsx
+++ b/src/main/resources/imports/docs/munkalap_sablon_uj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\work_hu\assets\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\private\work-hu-service\src\main\resources\imports\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896FBB98-EA44-40AE-BC40-270C1F32E3F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22FFA64-5248-4B02-AC79-C74FFD0C9094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11976" yWindow="204" windowWidth="10764" windowHeight="8976" xr2:uid="{3A8B3A12-02C8-4EB3-AD18-61BE7513E8CB}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{3A8B3A12-02C8-4EB3-AD18-61BE7513E8CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;Ft&quot;_-;\-* #,##0.00\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;Ft&quot;_-;\-* #,##0\ &quot;Ft&quot;_-;_-* &quot;-&quot;??\ &quot;Ft&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +88,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -461,16 +473,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,9 +535,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Pénznem" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -842,7 +856,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,437 +869,437 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="16" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="19"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="20"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="17" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="18" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="30"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="1"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="30"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="30"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="30"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="30"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="1"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="30"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="1"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="1"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="1"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="1"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="1"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="1"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="1"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="1"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="1"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="1"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="30"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="1"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="1"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="1"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="1"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="30"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="1"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="30"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="1"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="30"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="1"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="1"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="30"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="1"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="30"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="1"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="1"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="1"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="30"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="1"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="30"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="1"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="30"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="1"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="11"/>
-      <c r="B43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="1"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="11"/>
-      <c r="B44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="1"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="11"/>
-      <c r="B45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="1"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="30"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="11"/>
-      <c r="B46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="1"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="30"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="11"/>
-      <c r="B47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="1"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="30"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="11"/>
-      <c r="B48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="1"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="30"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="1"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="11"/>
-      <c r="B50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="1"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="30"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="11"/>
-      <c r="B51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="1"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="30"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="1"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="30"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="11"/>
-      <c r="B53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="1"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="30"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="11"/>
-      <c r="B54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="1"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="30"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="11"/>
-      <c r="B55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="1"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="30"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="11"/>
-      <c r="B56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="1"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="30"/>
     </row>
     <row r="57" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="12"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="3"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>